<commit_message>
remplissage de l'auto évaluation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Documents\Cours\BA5\AMT\Teaching-HEIGVD-AMT-2015-Project\evaluation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25356" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -233,8 +241,44 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -562,18 +606,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="97.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="97.796875" customWidth="1"/>
+    <col min="4" max="4" width="19.796875" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D1" s="3" t="s">
         <v>45</v>
       </c>
@@ -581,60 +625,78 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45">
+    <row r="3" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -647,127 +709,169 @@
         <v>0.16216216216216217</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="30">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="30">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="30">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="30">
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="30">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="30">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="30">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="30">
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -780,87 +884,114 @@
         <v>0.3783783783783784</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="30">
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="30">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -873,79 +1004,103 @@
         <v>0.24324324324324326</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="30">
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="30">
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="30">
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -958,10 +1113,10 @@
         <v>0.21621621621621623</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
@@ -970,16 +1125,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
@@ -988,7 +1143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>